<commit_message>
Updated the pipes sheet with additional columns
</commit_message>
<xml_diff>
--- a/gas_net/data/data_files/GasLib_11/networkData.xlsx
+++ b/gas_net/data/data_files/GasLib_11/networkData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nodes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pipes" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stations" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Arcs" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Nodes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Pipes" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Stations" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Arcs" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -737,7 +737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,6 +772,41 @@
           <t>roughness</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Nvol</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Direction</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>uMax</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>MMgas</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Tgas</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>xCH4</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -794,6 +829,9 @@
       <c r="F2" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -816,6 +854,9 @@
       <c r="F3" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -838,6 +879,9 @@
       <c r="F4" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -860,6 +904,9 @@
       <c r="F5" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -882,6 +929,9 @@
       <c r="F6" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -904,6 +954,9 @@
       <c r="F7" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -926,6 +979,9 @@
       <c r="F8" t="n">
         <v>0.0001</v>
       </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -947,6 +1003,9 @@
       </c>
       <c r="F9" t="n">
         <v>0.0001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data files with compressor map coefficients
</commit_message>
<xml_diff>
--- a/gas_net/data/data_files/GasLib_11/networkData.xlsx
+++ b/gas_net/data/data_files/GasLib_11/networkData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavinia\Documents\GitHub\gas_networks\gas_net\data\data_files\GasLib_11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssnaik\Biegler\gas_networks_italy\gas_networks\gas_net\data\data_files\GasLib_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE06F87-438D-4E37-AFE6-0245AFC6FBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E25F191-B9E8-47FD-AF1D-03F55320A951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>source</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Tgas</t>
+  </si>
+  <si>
+    <t>xCH4</t>
   </si>
   <si>
     <t>Z</t>
@@ -155,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,21 +170,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,18 +207,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,11 +516,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -557,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -577,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -597,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -617,7 +603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -640,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -660,7 +646,7 @@
         <v>-141</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -680,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -703,7 +689,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -726,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -746,7 +732,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -766,7 +752,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -793,15 +779,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="G1:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -818,22 +804,25 @@
       <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>55000</v>
@@ -850,22 +839,25 @@
       <c r="F2">
         <v>1E-4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" s="3">
-        <v>18</v>
-      </c>
-      <c r="I2" s="3">
-        <v>288</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="H2">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I2">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>55000</v>
@@ -882,22 +874,25 @@
       <c r="F3">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" s="3">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3">
-        <v>288</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="H3">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I3">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>55000</v>
@@ -914,22 +909,25 @@
       <c r="F4">
         <v>1E-4</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" s="3">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3">
-        <v>288</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="H4">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I4">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>55000</v>
@@ -946,22 +944,25 @@
       <c r="F5">
         <v>1E-4</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" s="3">
-        <v>18</v>
-      </c>
-      <c r="I5" s="3">
-        <v>288</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="H5">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I5">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J5">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>55000</v>
@@ -978,22 +979,25 @@
       <c r="F6">
         <v>1E-4</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" s="3">
-        <v>18</v>
-      </c>
-      <c r="I6" s="3">
-        <v>288</v>
-      </c>
-      <c r="J6" s="3">
+      <c r="H6">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I6">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J6">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>55000</v>
@@ -1010,22 +1014,25 @@
       <c r="F7">
         <v>1E-4</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7" s="3">
-        <v>18</v>
-      </c>
-      <c r="I7" s="3">
-        <v>288</v>
-      </c>
-      <c r="J7" s="3">
+      <c r="H7">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I7">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J7">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>55000</v>
@@ -1042,22 +1049,25 @@
       <c r="F8">
         <v>1E-4</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8" s="3">
-        <v>18</v>
-      </c>
-      <c r="I8" s="3">
-        <v>288</v>
-      </c>
-      <c r="J8" s="3">
+      <c r="H8">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I8">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J8">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>55000</v>
@@ -1074,17 +1084,20 @@
       <c r="F9">
         <v>1E-4</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9" s="3">
-        <v>18</v>
-      </c>
-      <c r="I9" s="3">
-        <v>288</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="H9">
+        <v>18.567399999999999</v>
+      </c>
+      <c r="I9">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="J9">
         <v>0.9</v>
+      </c>
+      <c r="K9">
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -1096,28 +1109,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>4000000</v>
@@ -1129,9 +1144,9 @@
         <v>180853756.58379799</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>4000000</v>
@@ -1154,20 +1169,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -1176,9 +1191,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1187,9 +1202,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1198,9 +1213,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1209,9 +1224,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1220,9 +1235,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -1231,9 +1246,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1242,9 +1257,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1253,9 +1268,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1264,9 +1279,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>

</xml_diff>